<commit_message>
aikavaativuustestailua, A* uusi heuristiikka, lisäyksiä gui:hin
</commit_message>
<xml_diff>
--- a/Dokumentaatio/Aikavaativuustestaus.xlsx
+++ b/Dokumentaatio/Aikavaativuustestaus.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Joonas\Documents\GitHub\labyrintin-ratkaisija\Dokumentaatio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\labyrintin-ratkaisija\Dokumentaatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Prim" sheetId="1" r:id="rId1"/>
@@ -189,7 +189,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -618,7 +618,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -656,7 +656,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -777,7 +777,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -815,7 +815,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -867,7 +867,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -897,7 +897,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -981,7 +981,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1412,7 +1412,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1450,7 +1450,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -1566,7 +1566,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1604,7 +1604,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -1656,7 +1656,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1686,7 +1686,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1770,7 +1770,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2196,7 +2196,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2234,7 +2234,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -2350,7 +2350,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2388,7 +2388,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -2440,7 +2440,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2470,7 +2470,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2554,7 +2554,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2985,7 +2985,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3023,7 +3023,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -3139,7 +3139,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3177,7 +3177,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -3229,7 +3229,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3259,7 +3259,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3343,7 +3343,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3891,7 +3891,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3929,7 +3929,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -4051,7 +4051,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4089,7 +4089,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -4141,7 +4141,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4171,7 +4171,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4255,7 +4255,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4772,7 +4772,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4810,7 +4810,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -4926,7 +4926,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4964,7 +4964,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -5016,7 +5016,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5046,7 +5046,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5130,7 +5130,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5541,7 +5541,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5579,7 +5579,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -5700,7 +5700,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5738,7 +5738,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -5790,7 +5790,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5820,7 +5820,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5904,7 +5904,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6405,7 +6405,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6443,7 +6443,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -6559,7 +6559,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6597,7 +6597,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -6649,7 +6649,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6679,7 +6679,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6763,7 +6763,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7156,7 +7156,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7194,7 +7194,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -7315,7 +7315,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7353,7 +7353,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -7405,7 +7405,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7435,7 +7435,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7519,7 +7519,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7937,7 +7937,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7975,7 +7975,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -8091,7 +8091,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8129,7 +8129,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -8181,7 +8181,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -8211,7 +8211,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8295,7 +8295,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8726,7 +8726,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8764,7 +8764,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -8880,7 +8880,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8918,7 +8918,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -8970,7 +8970,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9000,7 +9000,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9084,7 +9084,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9510,7 +9510,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9548,7 +9548,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541877968"/>
@@ -9664,7 +9664,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fi-FI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9702,7 +9702,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="541880264"/>
@@ -9754,7 +9754,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fi-FI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9784,7 +9784,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fi-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -16435,16 +16435,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>125730</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>135255</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>39330</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>48855</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>140610</xdr:rowOff>
+      <xdr:rowOff>64410</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16472,8 +16472,8 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:absoluteAnchor>
-    <xdr:pos x="70486" y="1638300"/>
-    <xdr:ext cx="5400000" cy="2880000"/>
+    <xdr:pos x="70486" y="1638299"/>
+    <xdr:ext cx="5400000" cy="3000375"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="17" name="Kaavio 16">
@@ -17126,18 +17126,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17157,7 +17157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -17177,7 +17177,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -17197,7 +17197,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10000</v>
       </c>
@@ -17217,7 +17217,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100000</v>
       </c>
@@ -17237,7 +17237,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1000000</v>
       </c>
@@ -17257,7 +17257,7 @@
         <v>2260</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10000000</v>
       </c>
@@ -17277,7 +17277,7 @@
         <v>7098</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>100000000</v>
       </c>
@@ -17312,15 +17312,15 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17340,7 +17340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -17360,7 +17360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -17380,7 +17380,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10000</v>
       </c>
@@ -17400,7 +17400,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100000</v>
       </c>
@@ -17420,7 +17420,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1000000</v>
       </c>
@@ -17440,7 +17440,7 @@
         <v>5560</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10000000</v>
       </c>
@@ -17474,13 +17474,13 @@
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17500,7 +17500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -17520,7 +17520,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -17540,7 +17540,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10000</v>
       </c>
@@ -17560,7 +17560,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100000</v>
       </c>
@@ -17580,7 +17580,7 @@
         <v>7298</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1000000</v>
       </c>
@@ -17614,7 +17614,7 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17629,7 +17629,7 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17640,11 +17640,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>